<commit_message>
made changes to input list added sql test
</commit_message>
<xml_diff>
--- a/Book2.xlsx
+++ b/Book2.xlsx
@@ -501,10 +501,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr filterMode="1"/>
   <dimension ref="A1:E41"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
@@ -534,7 +533,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="2" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -548,7 +547,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>17</v>
       </c>
@@ -565,7 +564,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>17</v>
       </c>
@@ -582,7 +581,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>17</v>
       </c>
@@ -599,7 +598,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A6" s="2" t="s">
         <v>17</v>
       </c>
@@ -616,7 +615,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="7" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>17</v>
       </c>
@@ -633,7 +632,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>17</v>
       </c>
@@ -650,7 +649,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>17</v>
       </c>
@@ -667,7 +666,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>17</v>
       </c>
@@ -684,7 +683,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>17</v>
       </c>
@@ -729,7 +728,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>6</v>
       </c>
@@ -771,7 +770,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="17" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>17</v>
       </c>
@@ -788,7 +787,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>17</v>
       </c>
@@ -805,7 +804,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>17</v>
       </c>
@@ -907,7 +906,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="26" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A26" s="1" t="s">
         <v>3</v>
       </c>
@@ -924,7 +923,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A27" s="1" t="s">
         <v>3</v>
       </c>
@@ -941,7 +940,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A28" s="1" t="s">
         <v>3</v>
       </c>
@@ -958,7 +957,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A29" s="1" t="s">
         <v>3</v>
       </c>
@@ -975,7 +974,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A30" s="1" t="s">
         <v>3</v>
       </c>
@@ -992,7 +991,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A31" s="1" t="s">
         <v>3</v>
       </c>
@@ -1009,7 +1008,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A32" s="1" t="s">
         <v>3</v>
       </c>
@@ -1026,7 +1025,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A33" s="1" t="s">
         <v>3</v>
       </c>
@@ -1043,7 +1042,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A34" s="1" t="s">
         <v>3</v>
       </c>
@@ -1060,7 +1059,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A35" s="1" t="s">
         <v>3</v>
       </c>
@@ -1077,7 +1076,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A36" s="1" t="s">
         <v>3</v>
       </c>
@@ -1094,7 +1093,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A37" s="1" t="s">
         <v>3</v>
       </c>
@@ -1111,7 +1110,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A38" s="1" t="s">
         <v>3</v>
       </c>
@@ -1128,7 +1127,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A39" s="1" t="s">
         <v>3</v>
       </c>
@@ -1145,7 +1144,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A40" s="1" t="s">
         <v>3</v>
       </c>
@@ -1162,7 +1161,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A41" s="1" t="s">
         <v>3</v>
       </c>
@@ -1180,28 +1179,13 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:E41">
-    <filterColumn colId="3">
-      <filters>
-        <filter val="ALL"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="A1:E41"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="200" verticalDpi="200" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101008F9A4161EA500A4C82B491574487E383" ma:contentTypeVersion="12" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="cbdf27a2e7bb0cda113f691274120128">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="3844b8d3-abe4-4d53-9885-598f7f5968e9" xmlns:ns4="ece5eda8-e753-47e2-b8e3-baa593ba0906" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="44f94028078e6778a54268945eec1755" ns3:_="" ns4:_="">
     <xsd:import namespace="3844b8d3-abe4-4d53-9885-598f7f5968e9"/>
@@ -1418,6 +1402,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement/>
@@ -1425,14 +1418,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AE461351-54C0-43A4-B6DC-5376C030C0D3}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B765C67F-B9E6-42DC-B564-BD1C8750B189}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1447,6 +1432,14 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AE461351-54C0-43A4-B6DC-5376C030C0D3}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>